<commit_message>
Done giao diện + Phân công nhiệm vụ
</commit_message>
<xml_diff>
--- a/TaskManager.xlsx
+++ b/TaskManager.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -13,10 +13,62 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Thái Trung Đức</t>
+  </si>
+  <si>
+    <t>Lê Chiêu Quốc</t>
+  </si>
+  <si>
+    <t>Bùi Hữu Quý</t>
+  </si>
+  <si>
+    <t>Phạm Như Ngọc Tuấn</t>
+  </si>
+  <si>
+    <t>Tuần 1</t>
+  </si>
+  <si>
+    <t>Tuần 2</t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện Mockup</t>
+  </si>
+  <si>
+    <t>Vẽ System UseCase Diagram</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về đấu giá, đấu giá online(Khái niệm, quy trình, các chức năng cơ bản)</t>
+  </si>
+  <si>
+    <t>Họp nhóm: Chọn đề tài, phân tích chức năng, viết Requirement Outline</t>
+  </si>
+  <si>
+    <t>Viết tài liệu SRS</t>
+  </si>
+  <si>
+    <t>Vẽ System Pages Flow</t>
+  </si>
+  <si>
+    <t>Họp nhóm: Phân tích cụ thể từng chức năng, người sử dụng, luồng hoạt động của website =&gt; đặc tả chức năng</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -44,14 +96,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +173,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +208,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +416,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>